<commit_message>
S4Loader - added option to generate just Floc uxl (self contained just needs a worklist, doesn't need PDTs or AIB exports).
</commit_message>
<xml_diff>
--- a/data/S4Loader_configs/pdt_field_value_enum_specifications.xlsx
+++ b/data/S4Loader_configs/pdt_field_value_enum_specifications.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\coding\work\work-flix\data\S4Loader_configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7B2E4A-E378-4E0A-82BF-7D23BD6D4D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5B509F-979C-489B-A8F9-06D156C4862D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49EDCC81-6B2D-486F-89E8-61367B638C15}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{49EDCC81-6B2D-486F-89E8-61367B638C15}"/>
   </bookViews>
   <sheets>
     <sheet name="PDT_Tank Data" sheetId="1" r:id="rId1"/>
+    <sheet name="PDT_Valves" sheetId="2" r:id="rId2"/>
+    <sheet name="PDT_Pressure Transmitter" sheetId="3" r:id="rId3"/>
+    <sheet name="PDT_Level Transmitter Data" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="296">
   <si>
     <t>Column Material</t>
   </si>
@@ -524,6 +527,405 @@
   </si>
   <si>
     <t>SHRSBM</t>
+  </si>
+  <si>
+    <t>Process Medium</t>
+  </si>
+  <si>
+    <t>Air</t>
+  </si>
+  <si>
+    <t>Activated Sludge</t>
+  </si>
+  <si>
+    <t>Sodium Hydroxide, 22.5%</t>
+  </si>
+  <si>
+    <t>Digested Sludge (3-5%)</t>
+  </si>
+  <si>
+    <t>Final Effluent</t>
+  </si>
+  <si>
+    <t>Ferric Sulphate</t>
+  </si>
+  <si>
+    <t>Humus Sludge</t>
+  </si>
+  <si>
+    <t>Industrial Effluent</t>
+  </si>
+  <si>
+    <t>Mixed Liquor (0.3-0.8%)</t>
+  </si>
+  <si>
+    <t>Primary Treated Effluent</t>
+  </si>
+  <si>
+    <t>Raw Sewage</t>
+  </si>
+  <si>
+    <t>Raw Sludge</t>
+  </si>
+  <si>
+    <t>Screened Raw Sewage</t>
+  </si>
+  <si>
+    <t>Secondary Treated Effluent</t>
+  </si>
+  <si>
+    <t>Thickened Sludge (2-5%)</t>
+  </si>
+  <si>
+    <t>Storm Flow</t>
+  </si>
+  <si>
+    <t>Limed Sludge Cake (up to 25%)</t>
+  </si>
+  <si>
+    <t>SEWAGE</t>
+  </si>
+  <si>
+    <t>AIR</t>
+  </si>
+  <si>
+    <t>Supply Voltage Units</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>VAC</t>
+  </si>
+  <si>
+    <t>VDC</t>
+  </si>
+  <si>
+    <t>Range Unit</t>
+  </si>
+  <si>
+    <t>BAR</t>
+  </si>
+  <si>
+    <t>BARG</t>
+  </si>
+  <si>
+    <t>CM/S</t>
+  </si>
+  <si>
+    <t>DEG C</t>
+  </si>
+  <si>
+    <t>IN H2O</t>
+  </si>
+  <si>
+    <t>IN WG</t>
+  </si>
+  <si>
+    <t>KPA</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>M H2O</t>
+  </si>
+  <si>
+    <t>M WG</t>
+  </si>
+  <si>
+    <t>M3/H</t>
+  </si>
+  <si>
+    <t>MBAR</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>MM H2O</t>
+  </si>
+  <si>
+    <t>MM WG</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>PCT</t>
+  </si>
+  <si>
+    <t>PSI</t>
+  </si>
+  <si>
+    <t>Output Signal Type</t>
+  </si>
+  <si>
+    <t>-1 - 10</t>
+  </si>
+  <si>
+    <t>-1 - 10 DIGITAL</t>
+  </si>
+  <si>
+    <t>0 - 1</t>
+  </si>
+  <si>
+    <t>0 - 1 DIGITAL</t>
+  </si>
+  <si>
+    <t>0 - 10</t>
+  </si>
+  <si>
+    <t>0 - 20 MA</t>
+  </si>
+  <si>
+    <t>0 - 24 MA</t>
+  </si>
+  <si>
+    <t>0 - 24000 MV</t>
+  </si>
+  <si>
+    <t>0 - 250 MV</t>
+  </si>
+  <si>
+    <t>250 MA</t>
+  </si>
+  <si>
+    <t>4 - 20 MA</t>
+  </si>
+  <si>
+    <t>4 - 20 MA HART</t>
+  </si>
+  <si>
+    <t>4 - 20 MV</t>
+  </si>
+  <si>
+    <t>4 - 24 MA</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>DIGITAL</t>
+  </si>
+  <si>
+    <t>DIGITAL PROFIBUS PA</t>
+  </si>
+  <si>
+    <t>DISCRETE</t>
+  </si>
+  <si>
+    <t>HART</t>
+  </si>
+  <si>
+    <t>PROFIBUS PA</t>
+  </si>
+  <si>
+    <t>0 - 24 MV</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>VAC/VDC</t>
+  </si>
+  <si>
+    <t>0 - 1 MA</t>
+  </si>
+  <si>
+    <t>10 - 10.5 MA</t>
+  </si>
+  <si>
+    <t>0 - 20 MV</t>
+  </si>
+  <si>
+    <t>0 - 200 MA</t>
+  </si>
+  <si>
+    <t>0 - 4 MA</t>
+  </si>
+  <si>
+    <t>1 - 0 DIGITAL</t>
+  </si>
+  <si>
+    <t>1 V/F</t>
+  </si>
+  <si>
+    <t>15 - 20 MA</t>
+  </si>
+  <si>
+    <t>2 - 20 MA</t>
+  </si>
+  <si>
+    <t>20 - 40 MA</t>
+  </si>
+  <si>
+    <t>4 - 100 MA</t>
+  </si>
+  <si>
+    <t>4 MA</t>
+  </si>
+  <si>
+    <t>44.2 MA</t>
+  </si>
+  <si>
+    <t>5 - 200 MA</t>
+  </si>
+  <si>
+    <t>PROFIBUS</t>
+  </si>
+  <si>
+    <t>PROFIBUS DP</t>
+  </si>
+  <si>
+    <t>0 - 10.5 MA</t>
+  </si>
+  <si>
+    <t>Output Type</t>
+  </si>
+  <si>
+    <t>ANALOGUE</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>barg</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>cm/s</t>
+  </si>
+  <si>
+    <t>ft</t>
+  </si>
+  <si>
+    <t>g/cm2</t>
+  </si>
+  <si>
+    <t>g/cm3</t>
+  </si>
+  <si>
+    <t>Kohm</t>
+  </si>
+  <si>
+    <t>l/h</t>
+  </si>
+  <si>
+    <t>l/s</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>m H2O</t>
+  </si>
+  <si>
+    <t>m WG</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>m3/h</t>
+  </si>
+  <si>
+    <t>mA</t>
+  </si>
+  <si>
+    <t>mbar</t>
+  </si>
+  <si>
+    <t>mg</t>
+  </si>
+  <si>
+    <t>mg/l</t>
+  </si>
+  <si>
+    <t>ml/d</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>ohm</t>
+  </si>
+  <si>
+    <t>pF</t>
+  </si>
+  <si>
+    <t>PPM</t>
+  </si>
+  <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>TCMD</t>
+  </si>
+  <si>
+    <t>uS/cm</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>G/CM2</t>
+  </si>
+  <si>
+    <t>G/CM3</t>
+  </si>
+  <si>
+    <t>KOHM</t>
+  </si>
+  <si>
+    <t>L/H</t>
+  </si>
+  <si>
+    <t>L/S</t>
+  </si>
+  <si>
+    <t>M/S</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>MG/L</t>
+  </si>
+  <si>
+    <t>ML/D</t>
+  </si>
+  <si>
+    <t>OHM</t>
+  </si>
+  <si>
+    <t>PF</t>
+  </si>
+  <si>
+    <t>US/CM</t>
+  </si>
+  <si>
+    <t>Set to Snort</t>
   </si>
 </sst>
 </file>
@@ -559,8 +961,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -877,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A74BCD5-CEE4-4AAF-BEF5-7858C3DBBFB4}">
   <dimension ref="A1:C176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2620,4 +3023,1368 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5581E532-3C2A-4F7C-A706-6F562035FAFB}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>163</v>
+      </c>
+      <c r="B14" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>163</v>
+      </c>
+      <c r="B18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E72F9188-74E3-4A3D-A9EC-3365854EE5BF}">
+  <dimension ref="A1:C41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" t="s">
+        <v>196</v>
+      </c>
+      <c r="C11" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>188</v>
+      </c>
+      <c r="B12" t="s">
+        <v>197</v>
+      </c>
+      <c r="C12" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B13" t="s">
+        <v>198</v>
+      </c>
+      <c r="C13" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B14" t="s">
+        <v>199</v>
+      </c>
+      <c r="C14" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>188</v>
+      </c>
+      <c r="B15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B16" t="s">
+        <v>201</v>
+      </c>
+      <c r="C16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B18" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>188</v>
+      </c>
+      <c r="B19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>188</v>
+      </c>
+      <c r="B20" t="s">
+        <v>205</v>
+      </c>
+      <c r="C20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>188</v>
+      </c>
+      <c r="B21" t="s">
+        <v>206</v>
+      </c>
+      <c r="C21" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>207</v>
+      </c>
+      <c r="B22" t="s">
+        <v>208</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>207</v>
+      </c>
+      <c r="B23" t="s">
+        <v>209</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>207</v>
+      </c>
+      <c r="B24" t="s">
+        <v>210</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B25" t="s">
+        <v>211</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>207</v>
+      </c>
+      <c r="B26" t="s">
+        <v>212</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>207</v>
+      </c>
+      <c r="B27" t="s">
+        <v>213</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>207</v>
+      </c>
+      <c r="B28" t="s">
+        <v>214</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>207</v>
+      </c>
+      <c r="B29" t="s">
+        <v>215</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>207</v>
+      </c>
+      <c r="B30" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>207</v>
+      </c>
+      <c r="B31" t="s">
+        <v>217</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>207</v>
+      </c>
+      <c r="B32" t="s">
+        <v>218</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>207</v>
+      </c>
+      <c r="B33" t="s">
+        <v>219</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>207</v>
+      </c>
+      <c r="B34" t="s">
+        <v>220</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>207</v>
+      </c>
+      <c r="B35" t="s">
+        <v>221</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>207</v>
+      </c>
+      <c r="B36" t="s">
+        <v>222</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>207</v>
+      </c>
+      <c r="B37" t="s">
+        <v>223</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>207</v>
+      </c>
+      <c r="B38" t="s">
+        <v>224</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>207</v>
+      </c>
+      <c r="B39" t="s">
+        <v>225</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>207</v>
+      </c>
+      <c r="B40" t="s">
+        <v>226</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>207</v>
+      </c>
+      <c r="B41" t="s">
+        <v>227</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F04C9B3-5E77-40CB-A3E9-FF9E8CE9BB9C}">
+  <dimension ref="A1:C62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8" t="s">
+        <v>231</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" t="s">
+        <v>232</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>207</v>
+      </c>
+      <c r="B10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" t="s">
+        <v>233</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>207</v>
+      </c>
+      <c r="B12" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>207</v>
+      </c>
+      <c r="B13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B14" t="s">
+        <v>236</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>207</v>
+      </c>
+      <c r="B15" t="s">
+        <v>237</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>207</v>
+      </c>
+      <c r="B16" t="s">
+        <v>238</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>207</v>
+      </c>
+      <c r="B17" t="s">
+        <v>239</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>207</v>
+      </c>
+      <c r="B18" t="s">
+        <v>240</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>207</v>
+      </c>
+      <c r="B19" t="s">
+        <v>241</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B20" t="s">
+        <v>218</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>207</v>
+      </c>
+      <c r="B21" t="s">
+        <v>220</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>207</v>
+      </c>
+      <c r="B22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>207</v>
+      </c>
+      <c r="B23" t="s">
+        <v>242</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>207</v>
+      </c>
+      <c r="B24" t="s">
+        <v>243</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B25" t="s">
+        <v>244</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>207</v>
+      </c>
+      <c r="B26" t="s">
+        <v>245</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>207</v>
+      </c>
+      <c r="B27" t="s">
+        <v>246</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>207</v>
+      </c>
+      <c r="B28" t="s">
+        <v>227</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>248</v>
+      </c>
+      <c r="B29" t="s">
+        <v>249</v>
+      </c>
+      <c r="C29" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>248</v>
+      </c>
+      <c r="B30" t="s">
+        <v>223</v>
+      </c>
+      <c r="C30" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>188</v>
+      </c>
+      <c r="B31" t="s">
+        <v>250</v>
+      </c>
+      <c r="C31" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>188</v>
+      </c>
+      <c r="B32" t="s">
+        <v>251</v>
+      </c>
+      <c r="C32" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>188</v>
+      </c>
+      <c r="B33" t="s">
+        <v>252</v>
+      </c>
+      <c r="C33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>188</v>
+      </c>
+      <c r="B34" t="s">
+        <v>253</v>
+      </c>
+      <c r="C34" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>188</v>
+      </c>
+      <c r="B35" t="s">
+        <v>254</v>
+      </c>
+      <c r="C35" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>188</v>
+      </c>
+      <c r="B36" t="s">
+        <v>255</v>
+      </c>
+      <c r="C36" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>188</v>
+      </c>
+      <c r="B37" t="s">
+        <v>256</v>
+      </c>
+      <c r="C37" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>188</v>
+      </c>
+      <c r="B38" t="s">
+        <v>257</v>
+      </c>
+      <c r="C38" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>188</v>
+      </c>
+      <c r="B39" t="s">
+        <v>258</v>
+      </c>
+      <c r="C39" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>188</v>
+      </c>
+      <c r="B40" t="s">
+        <v>259</v>
+      </c>
+      <c r="C40" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>188</v>
+      </c>
+      <c r="B41" t="s">
+        <v>260</v>
+      </c>
+      <c r="C41" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>188</v>
+      </c>
+      <c r="B42" t="s">
+        <v>261</v>
+      </c>
+      <c r="C42" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>188</v>
+      </c>
+      <c r="B43" t="s">
+        <v>262</v>
+      </c>
+      <c r="C43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>188</v>
+      </c>
+      <c r="B44" t="s">
+        <v>263</v>
+      </c>
+      <c r="C44" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>188</v>
+      </c>
+      <c r="B45" t="s">
+        <v>264</v>
+      </c>
+      <c r="C45" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>188</v>
+      </c>
+      <c r="B46" t="s">
+        <v>265</v>
+      </c>
+      <c r="C46" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>188</v>
+      </c>
+      <c r="B47" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>188</v>
+      </c>
+      <c r="B48" t="s">
+        <v>267</v>
+      </c>
+      <c r="C48" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>188</v>
+      </c>
+      <c r="B49" t="s">
+        <v>268</v>
+      </c>
+      <c r="C49" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>188</v>
+      </c>
+      <c r="B50" t="s">
+        <v>269</v>
+      </c>
+      <c r="C50" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>188</v>
+      </c>
+      <c r="B51" t="s">
+        <v>270</v>
+      </c>
+      <c r="C51" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>188</v>
+      </c>
+      <c r="B52" t="s">
+        <v>271</v>
+      </c>
+      <c r="C52" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>188</v>
+      </c>
+      <c r="B53" t="s">
+        <v>272</v>
+      </c>
+      <c r="C53" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>188</v>
+      </c>
+      <c r="B54" t="s">
+        <v>273</v>
+      </c>
+      <c r="C54" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>188</v>
+      </c>
+      <c r="B55" t="s">
+        <v>274</v>
+      </c>
+      <c r="C55" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>188</v>
+      </c>
+      <c r="B56" t="s">
+        <v>275</v>
+      </c>
+      <c r="C56" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>188</v>
+      </c>
+      <c r="B57" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>188</v>
+      </c>
+      <c r="B58" t="s">
+        <v>277</v>
+      </c>
+      <c r="C58" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>188</v>
+      </c>
+      <c r="B59" t="s">
+        <v>278</v>
+      </c>
+      <c r="C59" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>188</v>
+      </c>
+      <c r="B60" t="s">
+        <v>279</v>
+      </c>
+      <c r="C60" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>295</v>
+      </c>
+      <c r="B61" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>295</v>
+      </c>
+      <c r="B62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>